<commit_message>
updating tables for database
</commit_message>
<xml_diff>
--- a/y-Manipulated Tables/DataSet/Tables v2/FOREST_MINISTRY.xlsx
+++ b/y-Manipulated Tables/DataSet/Tables v2/FOREST_MINISTRY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New folder\Semester\8\CSE303-DBMS\DataSet\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BDSM\CSE303-sec-03-Group-03\y-Manipulated Tables\DataSet\Tables v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CA56AB-644A-4119-8833-FC23312B1E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D0CA1F-333A-48A5-8DD8-F7060BDE4AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
-  <si>
-    <t>ministryName</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>fm001</t>
   </si>
@@ -92,6 +86,12 @@
   </si>
   <si>
     <t>Forest Ministry</t>
+  </si>
+  <si>
+    <t>ministryID</t>
+  </si>
+  <si>
+    <t>locationID</t>
   </si>
 </sst>
 </file>
@@ -412,149 +412,146 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>